<commit_message>
(etapa 2) Envio de artefato atualizado
</commit_message>
<xml_diff>
--- a/Processo/Avaliação/GRE-Avaliacao-Projeto.xlsx
+++ b/Processo/Avaliação/GRE-Avaliacao-Projeto.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="56">
   <si>
     <t>INSTRUÇÕES</t>
   </si>
@@ -297,9 +297,6 @@
     <t xml:space="preserve"> </t>
   </si>
   <si>
-    <t>Documento de Requisitos</t>
-  </si>
-  <si>
     <t>Plano de Projeto&gt;Seção 6&gt;Divisão 6.1(Recursos Humanos)</t>
   </si>
   <si>
@@ -324,17 +321,23 @@
     <t>Plano de Projeto&gt;Seção 11 (Canais de Comunicação)</t>
   </si>
   <si>
-    <t>DOR - Nível G MPS-BR&gt;Seção 6 (Referencias Cruzadas Complementares)</t>
-  </si>
-  <si>
     <t>NC5 - Nível G MPS-BR</t>
+  </si>
+  <si>
+    <t>Documento de Requisitos - Nível G MPS-BR&gt;Seção 7(Aceitação Formal)</t>
+  </si>
+  <si>
+    <t>Documento de Requisitos - Nível G MPS-BR</t>
+  </si>
+  <si>
+    <t>Documento de Requisitos - Nível G MPS-BR&gt;Seção 6 (Referencias Cruzadas Complementares)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="19">
+  <fonts count="21">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -448,6 +451,20 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <i/>
+      <u/>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="6">
     <fill>
@@ -743,7 +760,7 @@
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="51">
+  <cellXfs count="53">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -890,6 +907,10 @@
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="8" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="2" applyFont="1"/>
+    <xf numFmtId="0" fontId="20" fillId="3" borderId="8" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="180"/>
     </xf>
   </cellXfs>
   <cellStyles count="6">
@@ -1395,10 +1416,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D127"/>
+  <dimension ref="A1:F126"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A20" workbookViewId="0">
-      <selection activeCell="A30" sqref="A30"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="G32" sqref="G32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1444,7 +1465,7 @@
       <c r="A4" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="B4" s="39"/>
+      <c r="B4" s="52"/>
       <c r="C4" s="38"/>
       <c r="D4" s="38"/>
     </row>
@@ -1474,9 +1495,7 @@
       <c r="C7" s="49" t="s">
         <v>19</v>
       </c>
-      <c r="D7" s="14" t="s">
-        <v>19</v>
-      </c>
+      <c r="D7" s="49"/>
     </row>
     <row r="8" spans="1:4" ht="12.75">
       <c r="A8" s="15" t="s">
@@ -1484,61 +1503,65 @@
       </c>
       <c r="B8" s="14"/>
       <c r="C8" s="14"/>
-      <c r="D8" s="14" t="s">
+      <c r="D8" s="49" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="12.75">
       <c r="A9" s="15" t="s">
-        <v>45</v>
+        <v>54</v>
       </c>
       <c r="B9" s="14"/>
       <c r="C9" s="14"/>
-      <c r="D9" s="14" t="s">
+      <c r="D9" s="49" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="12.75">
-      <c r="A10" s="15"/>
-      <c r="B10" s="14"/>
-      <c r="C10" s="14"/>
-      <c r="D10" s="14"/>
-    </row>
-    <row r="11" spans="1:4" ht="12.75">
-      <c r="A11" s="16"/>
-      <c r="B11" s="17" t="s">
+      <c r="A10" s="16"/>
+      <c r="B10" s="17" t="s">
         <v>21</v>
       </c>
-      <c r="C11" s="18"/>
-      <c r="D11" s="18"/>
-    </row>
-    <row r="12" spans="1:4" ht="82.5" customHeight="1">
-      <c r="A12" s="13" t="s">
+      <c r="C10" s="18"/>
+      <c r="D10" s="18"/>
+    </row>
+    <row r="11" spans="1:4" ht="82.5" customHeight="1">
+      <c r="A11" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="B12" s="39"/>
-      <c r="C12" s="37"/>
-      <c r="D12" s="37"/>
+      <c r="B11" s="39"/>
+      <c r="C11" s="37"/>
+      <c r="D11" s="37"/>
+    </row>
+    <row r="12" spans="1:4" ht="12.75">
+      <c r="A12" s="48" t="s">
+        <v>38</v>
+      </c>
+      <c r="B12" s="47"/>
+      <c r="C12" s="49" t="s">
+        <v>19</v>
+      </c>
+      <c r="D12" s="14"/>
     </row>
     <row r="13" spans="1:4" ht="12.75">
       <c r="A13" s="48" t="s">
-        <v>38</v>
-      </c>
-      <c r="B13" s="47"/>
+        <v>42</v>
+      </c>
+      <c r="B13" s="14"/>
       <c r="C13" s="49" t="s">
         <v>19</v>
       </c>
       <c r="D13" s="14"/>
     </row>
     <row r="14" spans="1:4" ht="12.75">
-      <c r="A14" s="48" t="s">
-        <v>42</v>
+      <c r="A14" s="15" t="s">
+        <v>53</v>
       </c>
       <c r="B14" s="14"/>
-      <c r="C14" s="49" t="s">
-        <v>19</v>
-      </c>
-      <c r="D14" s="14"/>
+      <c r="C14" s="14"/>
+      <c r="D14" s="49" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="15" spans="1:4" ht="12.75">
       <c r="A15" s="15"/>
@@ -1552,31 +1575,36 @@
       <c r="C16" s="14"/>
       <c r="D16" s="14"/>
     </row>
-    <row r="17" spans="1:4" ht="12.75">
-      <c r="A17" s="15"/>
-      <c r="B17" s="14"/>
-      <c r="C17" s="14"/>
-      <c r="D17" s="14"/>
-    </row>
-    <row r="18" spans="1:4" ht="12.75">
-      <c r="A18" s="16"/>
-      <c r="B18" s="17" t="s">
+    <row r="17" spans="1:6" ht="12.75">
+      <c r="A17" s="16"/>
+      <c r="B17" s="17" t="s">
         <v>21</v>
       </c>
-      <c r="C18" s="18"/>
-      <c r="D18" s="18"/>
-    </row>
-    <row r="19" spans="1:4" ht="51">
-      <c r="A19" s="13" t="s">
+      <c r="C17" s="18"/>
+      <c r="D17" s="18"/>
+    </row>
+    <row r="18" spans="1:6" ht="51">
+      <c r="A18" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="B19" s="37"/>
-      <c r="C19" s="37"/>
-      <c r="D19" s="37"/>
-    </row>
-    <row r="20" spans="1:4" ht="12.75">
-      <c r="A20" s="48" t="s">
+      <c r="B18" s="37"/>
+      <c r="C18" s="37"/>
+      <c r="D18" s="37"/>
+    </row>
+    <row r="19" spans="1:6" ht="12.75">
+      <c r="A19" s="48" t="s">
         <v>38</v>
+      </c>
+      <c r="B19" s="14"/>
+      <c r="C19" s="49" t="s">
+        <v>19</v>
+      </c>
+      <c r="D19" s="14"/>
+      <c r="F19" s="51"/>
+    </row>
+    <row r="20" spans="1:6" ht="12.75">
+      <c r="A20" s="15" t="s">
+        <v>24</v>
       </c>
       <c r="B20" s="14"/>
       <c r="C20" s="49" t="s">
@@ -1584,111 +1612,111 @@
       </c>
       <c r="D20" s="14"/>
     </row>
-    <row r="21" spans="1:4" ht="12.75">
+    <row r="21" spans="1:6" ht="12.75">
       <c r="A21" s="15" t="s">
-        <v>24</v>
+        <v>55</v>
       </c>
       <c r="B21" s="14"/>
-      <c r="C21" s="49" t="s">
-        <v>19</v>
-      </c>
-      <c r="D21" s="14"/>
-    </row>
-    <row r="22" spans="1:4" ht="12.75">
-      <c r="A22" s="15" t="s">
-        <v>53</v>
-      </c>
+      <c r="C21" s="14"/>
+      <c r="D21" s="49" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" ht="12.75">
+      <c r="A22" s="15"/>
       <c r="B22" s="14"/>
       <c r="C22" s="14"/>
-      <c r="D22" s="14" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" ht="12.75">
+      <c r="D22" s="14"/>
+    </row>
+    <row r="23" spans="1:6" ht="12.75">
       <c r="A23" s="15"/>
       <c r="B23" s="14"/>
       <c r="C23" s="14"/>
       <c r="D23" s="14"/>
     </row>
-    <row r="24" spans="1:4" ht="12.75">
-      <c r="A24" s="15"/>
-      <c r="B24" s="14"/>
-      <c r="C24" s="14"/>
-      <c r="D24" s="14"/>
-    </row>
-    <row r="25" spans="1:4" ht="12.75">
-      <c r="A25" s="16"/>
-      <c r="B25" s="17" t="s">
+    <row r="24" spans="1:6" ht="12.75">
+      <c r="A24" s="16"/>
+      <c r="B24" s="17" t="s">
         <v>21</v>
       </c>
-      <c r="C25" s="18"/>
-      <c r="D25" s="18"/>
-    </row>
-    <row r="26" spans="1:4" ht="63.75">
-      <c r="A26" s="13" t="s">
+      <c r="C24" s="18"/>
+      <c r="D24" s="18"/>
+    </row>
+    <row r="25" spans="1:6" ht="63.75">
+      <c r="A25" s="13" t="s">
         <v>25</v>
       </c>
-      <c r="B26" s="37"/>
-      <c r="C26" s="37"/>
-      <c r="D26" s="37"/>
-    </row>
-    <row r="27" spans="1:4" ht="12.75">
-      <c r="A27" s="48" t="s">
+      <c r="B25" s="37"/>
+      <c r="C25" s="37"/>
+      <c r="D25" s="37"/>
+    </row>
+    <row r="26" spans="1:6" ht="12.75">
+      <c r="A26" s="48" t="s">
         <v>38</v>
       </c>
+      <c r="B26" s="14"/>
+      <c r="C26" s="49" t="s">
+        <v>19</v>
+      </c>
+      <c r="D26" s="14"/>
+    </row>
+    <row r="27" spans="1:6" ht="12.75">
+      <c r="A27" s="15" t="s">
+        <v>52</v>
+      </c>
       <c r="B27" s="14"/>
-      <c r="C27" s="49" t="s">
-        <v>19</v>
-      </c>
-      <c r="D27" s="14"/>
-    </row>
-    <row r="28" spans="1:4" ht="12.75">
-      <c r="A28" s="15" t="s">
-        <v>54</v>
-      </c>
+      <c r="C27" s="14"/>
+      <c r="D27" s="49" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" ht="12.75">
+      <c r="A28" s="15"/>
       <c r="B28" s="14"/>
       <c r="C28" s="14"/>
-      <c r="D28" s="14" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" ht="12.75">
+      <c r="D28" s="14"/>
+    </row>
+    <row r="29" spans="1:6" ht="12.75">
       <c r="A29" s="15"/>
       <c r="B29" s="14"/>
       <c r="C29" s="14"/>
       <c r="D29" s="14"/>
     </row>
-    <row r="30" spans="1:4" ht="12.75">
+    <row r="30" spans="1:6" ht="12.75">
       <c r="A30" s="15"/>
       <c r="B30" s="14"/>
       <c r="C30" s="14"/>
       <c r="D30" s="14"/>
     </row>
-    <row r="31" spans="1:4" ht="12.75">
-      <c r="A31" s="15"/>
-      <c r="B31" s="14"/>
-      <c r="C31" s="14"/>
-      <c r="D31" s="14"/>
-    </row>
-    <row r="32" spans="1:4" ht="12.75">
-      <c r="A32" s="16"/>
-      <c r="B32" s="17" t="s">
+    <row r="31" spans="1:6" ht="12.75">
+      <c r="A31" s="16"/>
+      <c r="B31" s="17" t="s">
         <v>21</v>
       </c>
-      <c r="C32" s="18"/>
-      <c r="D32" s="18"/>
-    </row>
-    <row r="33" spans="1:4" ht="63.75">
-      <c r="A33" s="13" t="s">
+      <c r="C31" s="18"/>
+      <c r="D31" s="18"/>
+    </row>
+    <row r="32" spans="1:6" ht="63.75">
+      <c r="A32" s="13" t="s">
         <v>26</v>
       </c>
-      <c r="B33" s="37"/>
-      <c r="C33" s="37"/>
-      <c r="D33" s="37"/>
+      <c r="B32" s="37"/>
+      <c r="C32" s="37"/>
+      <c r="D32" s="37"/>
+    </row>
+    <row r="33" spans="1:4" ht="12.75">
+      <c r="A33" s="48" t="s">
+        <v>38</v>
+      </c>
+      <c r="B33" s="14"/>
+      <c r="C33" s="49" t="s">
+        <v>19</v>
+      </c>
+      <c r="D33" s="14"/>
     </row>
     <row r="34" spans="1:4" ht="12.75">
-      <c r="A34" s="48" t="s">
-        <v>38</v>
+      <c r="A34" s="15" t="s">
+        <v>27</v>
       </c>
       <c r="B34" s="14"/>
       <c r="C34" s="49" t="s">
@@ -1698,18 +1726,16 @@
     </row>
     <row r="35" spans="1:4" ht="12.75">
       <c r="A35" s="15" t="s">
-        <v>27</v>
+        <v>45</v>
       </c>
       <c r="B35" s="14"/>
-      <c r="C35" s="49" t="s">
-        <v>19</v>
+      <c r="C35" s="14" t="s">
+        <v>43</v>
       </c>
       <c r="D35" s="14"/>
     </row>
     <row r="36" spans="1:4" ht="12.75">
-      <c r="A36" s="15" t="s">
-        <v>46</v>
-      </c>
+      <c r="A36" s="15"/>
       <c r="B36" s="14"/>
       <c r="C36" s="14" t="s">
         <v>43</v>
@@ -1719,82 +1745,80 @@
     <row r="37" spans="1:4" ht="12.75">
       <c r="A37" s="15"/>
       <c r="B37" s="14"/>
-      <c r="C37" s="14" t="s">
-        <v>43</v>
-      </c>
+      <c r="C37" s="14"/>
       <c r="D37" s="14"/>
     </row>
     <row r="38" spans="1:4" ht="12.75">
-      <c r="A38" s="15"/>
-      <c r="B38" s="14"/>
-      <c r="C38" s="14"/>
-      <c r="D38" s="14"/>
-    </row>
-    <row r="39" spans="1:4" ht="12.75">
-      <c r="A39" s="36"/>
-      <c r="B39" s="35" t="s">
+      <c r="A38" s="36"/>
+      <c r="B38" s="35" t="s">
         <v>21</v>
       </c>
-      <c r="C39" s="34"/>
-      <c r="D39" s="34"/>
+      <c r="C38" s="34"/>
+      <c r="D38" s="34"/>
+    </row>
+    <row r="39" spans="1:4" ht="15.75">
+      <c r="A39" s="19"/>
+      <c r="B39" s="20"/>
+      <c r="C39" s="20"/>
+      <c r="D39" s="20"/>
     </row>
     <row r="40" spans="1:4" ht="15.75">
-      <c r="A40" s="19"/>
-      <c r="B40" s="20"/>
-      <c r="C40" s="20"/>
-      <c r="D40" s="20"/>
+      <c r="A40" s="21" t="s">
+        <v>28</v>
+      </c>
+      <c r="B40" s="22"/>
+      <c r="C40" s="22"/>
+      <c r="D40" s="22"/>
     </row>
     <row r="41" spans="1:4" ht="15.75">
-      <c r="A41" s="21" t="s">
-        <v>28</v>
-      </c>
-      <c r="B41" s="22"/>
-      <c r="C41" s="22"/>
-      <c r="D41" s="22"/>
+      <c r="A41" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B41" s="23"/>
+      <c r="C41" s="24"/>
+      <c r="D41" s="24"/>
     </row>
     <row r="42" spans="1:4" ht="15.75">
-      <c r="A42" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="B42" s="23"/>
-      <c r="C42" s="24"/>
-      <c r="D42" s="24"/>
-    </row>
-    <row r="43" spans="1:4" ht="15.75">
-      <c r="A43" s="25" t="s">
+      <c r="A42" s="25" t="s">
         <v>29</v>
       </c>
-      <c r="B43" s="26"/>
-      <c r="C43" s="27"/>
-      <c r="D43" s="27"/>
-    </row>
-    <row r="44" spans="1:4" ht="63.75">
-      <c r="A44" s="28" t="s">
+      <c r="B42" s="26"/>
+      <c r="C42" s="27"/>
+      <c r="D42" s="27"/>
+    </row>
+    <row r="43" spans="1:4" ht="63.75">
+      <c r="A43" s="28" t="s">
         <v>30</v>
       </c>
-      <c r="B44" s="29"/>
-      <c r="C44" s="30"/>
-      <c r="D44" s="30"/>
+      <c r="B43" s="29"/>
+      <c r="C43" s="30"/>
+      <c r="D43" s="30"/>
+    </row>
+    <row r="44" spans="1:4" ht="12.75">
+      <c r="A44" s="48" t="s">
+        <v>39</v>
+      </c>
+      <c r="B44" s="14"/>
+      <c r="C44" s="49" t="s">
+        <v>19</v>
+      </c>
+      <c r="D44" s="14"/>
     </row>
     <row r="45" spans="1:4" ht="12.75">
-      <c r="A45" s="48" t="s">
-        <v>39</v>
+      <c r="A45" s="15" t="s">
+        <v>46</v>
       </c>
       <c r="B45" s="14"/>
-      <c r="C45" s="49" t="s">
-        <v>19</v>
-      </c>
-      <c r="D45" s="14"/>
+      <c r="C45" s="14"/>
+      <c r="D45" s="49" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="46" spans="1:4" ht="12.75">
-      <c r="A46" s="15" t="s">
-        <v>47</v>
-      </c>
+      <c r="A46" s="15"/>
       <c r="B46" s="14"/>
       <c r="C46" s="14"/>
-      <c r="D46" s="14" t="s">
-        <v>19</v>
-      </c>
+      <c r="D46" s="14"/>
     </row>
     <row r="47" spans="1:4" ht="12.75">
       <c r="A47" s="15"/>
@@ -1810,35 +1834,37 @@
     </row>
     <row r="49" spans="1:4" ht="12.75">
       <c r="A49" s="15"/>
-      <c r="B49" s="14"/>
-      <c r="C49" s="14"/>
-      <c r="D49" s="14"/>
-    </row>
-    <row r="50" spans="1:4" ht="12.75">
-      <c r="A50" s="15"/>
-      <c r="B50" s="17" t="s">
+      <c r="B49" s="17" t="s">
         <v>21</v>
       </c>
-      <c r="C50" s="18"/>
-      <c r="D50" s="18"/>
-    </row>
-    <row r="51" spans="1:4" ht="26.25">
-      <c r="A51" s="28" t="s">
+      <c r="C49" s="18"/>
+      <c r="D49" s="18"/>
+    </row>
+    <row r="50" spans="1:4" ht="26.25">
+      <c r="A50" s="28" t="s">
         <v>31</v>
       </c>
-      <c r="B51" s="31"/>
-      <c r="C51" s="32"/>
-      <c r="D51" s="32"/>
+      <c r="B50" s="31"/>
+      <c r="C50" s="32"/>
+      <c r="D50" s="32"/>
+    </row>
+    <row r="51" spans="1:4" ht="12.75">
+      <c r="A51" s="48" t="s">
+        <v>39</v>
+      </c>
+      <c r="B51" s="14"/>
+      <c r="C51" s="50" t="s">
+        <v>19</v>
+      </c>
+      <c r="D51" s="50"/>
     </row>
     <row r="52" spans="1:4" ht="12.75">
-      <c r="A52" s="48" t="s">
-        <v>39</v>
+      <c r="A52" s="15" t="s">
+        <v>47</v>
       </c>
       <c r="B52" s="14"/>
-      <c r="C52" s="50" t="s">
-        <v>19</v>
-      </c>
-      <c r="D52" s="50" t="s">
+      <c r="C52" s="14"/>
+      <c r="D52" s="49" t="s">
         <v>19</v>
       </c>
     </row>
@@ -1848,7 +1874,7 @@
       </c>
       <c r="B53" s="14"/>
       <c r="C53" s="14"/>
-      <c r="D53" s="14" t="s">
+      <c r="D53" s="49" t="s">
         <v>19</v>
       </c>
     </row>
@@ -1858,51 +1884,51 @@
       </c>
       <c r="B54" s="14"/>
       <c r="C54" s="14"/>
-      <c r="D54" s="14" t="s">
+      <c r="D54" s="49" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="55" spans="1:4" ht="12.75">
-      <c r="A55" s="15" t="s">
-        <v>50</v>
-      </c>
+      <c r="A55" s="15"/>
       <c r="B55" s="14"/>
       <c r="C55" s="14"/>
-      <c r="D55" s="14" t="s">
-        <v>19</v>
-      </c>
+      <c r="D55" s="14"/>
     </row>
     <row r="56" spans="1:4" ht="12.75">
       <c r="A56" s="15"/>
-      <c r="B56" s="14"/>
-      <c r="C56" s="14"/>
-      <c r="D56" s="14"/>
-    </row>
-    <row r="57" spans="1:4" ht="12.75">
-      <c r="A57" s="15"/>
-      <c r="B57" s="17" t="s">
+      <c r="B56" s="17" t="s">
         <v>21</v>
       </c>
-      <c r="C57" s="18"/>
-      <c r="D57" s="18"/>
-    </row>
-    <row r="58" spans="1:4" ht="64.5">
-      <c r="A58" s="28" t="s">
+      <c r="C56" s="18"/>
+      <c r="D56" s="18"/>
+    </row>
+    <row r="57" spans="1:4" ht="64.5">
+      <c r="A57" s="28" t="s">
         <v>32</v>
       </c>
-      <c r="B58" s="32"/>
-      <c r="C58" s="32"/>
-      <c r="D58" s="32"/>
+      <c r="B57" s="32"/>
+      <c r="C57" s="32"/>
+      <c r="D57" s="32"/>
+    </row>
+    <row r="58" spans="1:4" ht="12.75">
+      <c r="A58" s="48" t="s">
+        <v>38</v>
+      </c>
+      <c r="B58" s="14"/>
+      <c r="C58" s="49" t="s">
+        <v>19</v>
+      </c>
+      <c r="D58" s="14"/>
     </row>
     <row r="59" spans="1:4" ht="12.75">
-      <c r="A59" s="48" t="s">
-        <v>38</v>
+      <c r="A59" s="15" t="s">
+        <v>50</v>
       </c>
       <c r="B59" s="14"/>
-      <c r="C59" s="49" t="s">
-        <v>19</v>
-      </c>
-      <c r="D59" s="14"/>
+      <c r="C59" s="14"/>
+      <c r="D59" s="49" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="60" spans="1:4" ht="12.75">
       <c r="A60" s="15" t="s">
@@ -1910,19 +1936,15 @@
       </c>
       <c r="B60" s="14"/>
       <c r="C60" s="14"/>
-      <c r="D60" s="14" t="s">
+      <c r="D60" s="49" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="61" spans="1:4" ht="12.75">
-      <c r="A61" s="15" t="s">
-        <v>52</v>
-      </c>
+      <c r="A61" s="15"/>
       <c r="B61" s="14"/>
       <c r="C61" s="14"/>
-      <c r="D61" s="14" t="s">
-        <v>19</v>
-      </c>
+      <c r="D61" s="14"/>
     </row>
     <row r="62" spans="1:4" ht="12.75">
       <c r="A62" s="15"/>
@@ -1932,45 +1954,45 @@
     </row>
     <row r="63" spans="1:4" ht="12.75">
       <c r="A63" s="15"/>
-      <c r="B63" s="14"/>
-      <c r="C63" s="14"/>
-      <c r="D63" s="14"/>
-    </row>
-    <row r="64" spans="1:4" ht="12.75">
-      <c r="A64" s="15"/>
-      <c r="B64" s="17" t="s">
+      <c r="B63" s="17" t="s">
         <v>21</v>
       </c>
-      <c r="C64" s="18"/>
-      <c r="D64" s="18"/>
-    </row>
-    <row r="65" spans="1:4" ht="51.75">
-      <c r="A65" s="28" t="s">
+      <c r="C63" s="18"/>
+      <c r="D63" s="18"/>
+    </row>
+    <row r="64" spans="1:4" ht="51.75">
+      <c r="A64" s="28" t="s">
         <v>33</v>
       </c>
-      <c r="B65" s="32"/>
-      <c r="C65" s="32"/>
-      <c r="D65" s="32"/>
+      <c r="B64" s="32"/>
+      <c r="C64" s="32"/>
+      <c r="D64" s="32"/>
+    </row>
+    <row r="65" spans="1:4" ht="12.75">
+      <c r="A65" s="48" t="s">
+        <v>40</v>
+      </c>
+      <c r="B65" s="14"/>
+      <c r="C65" s="49" t="s">
+        <v>19</v>
+      </c>
+      <c r="D65" s="14"/>
     </row>
     <row r="66" spans="1:4" ht="12.75">
-      <c r="A66" s="48" t="s">
-        <v>40</v>
+      <c r="A66" s="15" t="s">
+        <v>44</v>
       </c>
       <c r="B66" s="14"/>
-      <c r="C66" s="49" t="s">
-        <v>19</v>
-      </c>
-      <c r="D66" s="14"/>
+      <c r="C66" s="14"/>
+      <c r="D66" s="49" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="67" spans="1:4" ht="12.75">
-      <c r="A67" s="15" t="s">
-        <v>45</v>
-      </c>
+      <c r="A67" s="15"/>
       <c r="B67" s="14"/>
       <c r="C67" s="14"/>
-      <c r="D67" s="14" t="s">
-        <v>19</v>
-      </c>
+      <c r="D67" s="14"/>
     </row>
     <row r="68" spans="1:4" ht="12.75">
       <c r="A68" s="15"/>
@@ -1986,47 +2008,47 @@
     </row>
     <row r="70" spans="1:4" ht="12.75">
       <c r="A70" s="15"/>
-      <c r="B70" s="14"/>
-      <c r="C70" s="14"/>
-      <c r="D70" s="14"/>
-    </row>
-    <row r="71" spans="1:4" ht="12.75">
-      <c r="A71" s="15"/>
-      <c r="B71" s="17" t="s">
+      <c r="B70" s="17" t="s">
         <v>21</v>
       </c>
-      <c r="C71" s="18"/>
-      <c r="D71" s="18"/>
-    </row>
-    <row r="72" spans="1:4" ht="64.5">
-      <c r="A72" s="28" t="s">
+      <c r="C70" s="18"/>
+      <c r="D70" s="18"/>
+    </row>
+    <row r="71" spans="1:4" ht="64.5">
+      <c r="A71" s="28" t="s">
         <v>34</v>
       </c>
-      <c r="B72" s="32"/>
-      <c r="C72" s="32"/>
-      <c r="D72" s="32"/>
+      <c r="B71" s="32"/>
+      <c r="C71" s="32"/>
+      <c r="D71" s="32"/>
+    </row>
+    <row r="72" spans="1:4" ht="12.75">
+      <c r="A72" s="48" t="s">
+        <v>40</v>
+      </c>
+      <c r="B72" s="14"/>
+      <c r="C72" s="49" t="s">
+        <v>19</v>
+      </c>
+      <c r="D72" s="49" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="73" spans="1:4" ht="12.75">
-      <c r="A73" s="48" t="s">
-        <v>40</v>
+      <c r="A73" s="15" t="s">
+        <v>44</v>
       </c>
       <c r="B73" s="14"/>
-      <c r="C73" s="49" t="s">
-        <v>19</v>
-      </c>
+      <c r="C73" s="14"/>
       <c r="D73" s="49" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="74" spans="1:4" ht="12.75">
-      <c r="A74" s="15" t="s">
-        <v>45</v>
-      </c>
+      <c r="A74" s="15"/>
       <c r="B74" s="14"/>
       <c r="C74" s="14"/>
-      <c r="D74" s="14" t="s">
-        <v>19</v>
-      </c>
+      <c r="D74" s="14"/>
     </row>
     <row r="75" spans="1:4" ht="12.75">
       <c r="A75" s="15"/>
@@ -2042,45 +2064,45 @@
     </row>
     <row r="77" spans="1:4" ht="12.75">
       <c r="A77" s="15"/>
-      <c r="B77" s="14"/>
-      <c r="C77" s="14"/>
-      <c r="D77" s="14"/>
-    </row>
-    <row r="78" spans="1:4" ht="12.75">
-      <c r="A78" s="15"/>
-      <c r="B78" s="17" t="s">
+      <c r="B77" s="17" t="s">
         <v>21</v>
       </c>
-      <c r="C78" s="18"/>
-      <c r="D78" s="18"/>
-    </row>
-    <row r="79" spans="1:4" ht="64.5">
-      <c r="A79" s="28" t="s">
+      <c r="C77" s="18"/>
+      <c r="D77" s="18"/>
+    </row>
+    <row r="78" spans="1:4" ht="64.5">
+      <c r="A78" s="28" t="s">
         <v>35</v>
       </c>
-      <c r="B79" s="32"/>
-      <c r="C79" s="32"/>
-      <c r="D79" s="32"/>
+      <c r="B78" s="32"/>
+      <c r="C78" s="32"/>
+      <c r="D78" s="32"/>
+    </row>
+    <row r="79" spans="1:4" ht="12.75">
+      <c r="A79" s="48" t="s">
+        <v>41</v>
+      </c>
+      <c r="B79" s="14"/>
+      <c r="C79" s="49" t="s">
+        <v>19</v>
+      </c>
+      <c r="D79" s="14"/>
     </row>
     <row r="80" spans="1:4" ht="12.75">
-      <c r="A80" s="48" t="s">
-        <v>41</v>
+      <c r="A80" s="15" t="s">
+        <v>49</v>
       </c>
       <c r="B80" s="14"/>
-      <c r="C80" s="49" t="s">
-        <v>19</v>
-      </c>
-      <c r="D80" s="14"/>
+      <c r="C80" s="14"/>
+      <c r="D80" s="49" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="81" spans="1:4" ht="12.75">
-      <c r="A81" s="15" t="s">
-        <v>50</v>
-      </c>
+      <c r="A81" s="15"/>
       <c r="B81" s="14"/>
       <c r="C81" s="14"/>
-      <c r="D81" s="14" t="s">
-        <v>19</v>
-      </c>
+      <c r="D81" s="14"/>
     </row>
     <row r="82" spans="1:4" ht="12.75">
       <c r="A82" s="15"/>
@@ -2096,57 +2118,57 @@
     </row>
     <row r="84" spans="1:4" ht="12.75">
       <c r="A84" s="15"/>
-      <c r="B84" s="14"/>
-      <c r="C84" s="14"/>
-      <c r="D84" s="14"/>
-    </row>
-    <row r="85" spans="1:4" ht="12.75">
-      <c r="A85" s="15"/>
-      <c r="B85" s="17" t="s">
+      <c r="B84" s="17" t="s">
         <v>21</v>
       </c>
-      <c r="C85" s="18"/>
-      <c r="D85" s="18"/>
-    </row>
-    <row r="86" spans="1:4" ht="51.75">
-      <c r="A86" s="28" t="s">
+      <c r="C84" s="18"/>
+      <c r="D84" s="18"/>
+    </row>
+    <row r="85" spans="1:4" ht="51.75">
+      <c r="A85" s="28" t="s">
         <v>36</v>
       </c>
-      <c r="B86" s="32"/>
-      <c r="C86" s="32"/>
-      <c r="D86" s="32"/>
+      <c r="B85" s="32"/>
+      <c r="C85" s="32"/>
+      <c r="D85" s="32"/>
+    </row>
+    <row r="86" spans="1:4" ht="12.75">
+      <c r="A86" s="48" t="s">
+        <v>38</v>
+      </c>
+      <c r="B86" s="14"/>
+      <c r="C86" s="49" t="s">
+        <v>19</v>
+      </c>
+      <c r="D86" s="14"/>
     </row>
     <row r="87" spans="1:4" ht="12.75">
       <c r="A87" s="48" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="B87" s="14"/>
       <c r="C87" s="49" t="s">
         <v>19</v>
       </c>
-      <c r="D87" s="14"/>
+      <c r="D87" s="49" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="88" spans="1:4" ht="12.75">
-      <c r="A88" s="48" t="s">
-        <v>41</v>
+      <c r="A88" s="15" t="s">
+        <v>49</v>
       </c>
       <c r="B88" s="14"/>
-      <c r="C88" s="49" t="s">
-        <v>19</v>
-      </c>
+      <c r="C88" s="14"/>
       <c r="D88" s="49" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="89" spans="1:4" ht="12.75">
-      <c r="A89" s="15" t="s">
-        <v>50</v>
-      </c>
+      <c r="A89" s="15"/>
       <c r="B89" s="14"/>
       <c r="C89" s="14"/>
-      <c r="D89" s="14" t="s">
-        <v>19</v>
-      </c>
+      <c r="D89" s="14"/>
     </row>
     <row r="90" spans="1:4" ht="12.75">
       <c r="A90" s="15"/>
@@ -2156,17 +2178,17 @@
     </row>
     <row r="91" spans="1:4" ht="12.75">
       <c r="A91" s="15"/>
-      <c r="B91" s="14"/>
-      <c r="C91" s="14"/>
-      <c r="D91" s="14"/>
+      <c r="B91" s="17" t="s">
+        <v>21</v>
+      </c>
+      <c r="C91" s="18"/>
+      <c r="D91" s="18"/>
     </row>
     <row r="92" spans="1:4" ht="12.75">
-      <c r="A92" s="15"/>
-      <c r="B92" s="17" t="s">
-        <v>21</v>
-      </c>
-      <c r="C92" s="18"/>
-      <c r="D92" s="18"/>
+      <c r="A92" s="7"/>
+      <c r="B92" s="7"/>
+      <c r="C92" s="7"/>
+      <c r="D92" s="7"/>
     </row>
     <row r="93" spans="1:4" ht="12.75">
       <c r="A93" s="7"/>
@@ -2252,13 +2274,13 @@
       <c r="C106" s="7"/>
       <c r="D106" s="7"/>
     </row>
-    <row r="107" spans="1:4" ht="12.75">
+    <row r="107" spans="1:4" ht="69.75" customHeight="1">
       <c r="A107" s="7"/>
       <c r="B107" s="7"/>
       <c r="C107" s="7"/>
       <c r="D107" s="7"/>
     </row>
-    <row r="108" spans="1:4" ht="69.75" customHeight="1">
+    <row r="108" spans="1:4" ht="12.75">
       <c r="A108" s="7"/>
       <c r="B108" s="7"/>
       <c r="C108" s="7"/>
@@ -2372,37 +2394,42 @@
       <c r="C126" s="7"/>
       <c r="D126" s="7"/>
     </row>
-    <row r="127" spans="1:4" ht="12.75">
-      <c r="A127" s="7"/>
-      <c r="B127" s="7"/>
-      <c r="C127" s="7"/>
-      <c r="D127" s="7"/>
-    </row>
   </sheetData>
   <phoneticPr fontId="0" type="noConversion"/>
   <hyperlinks>
     <hyperlink ref="C6" r:id="rId1"/>
-    <hyperlink ref="C13" r:id="rId2"/>
-    <hyperlink ref="C20" r:id="rId3"/>
-    <hyperlink ref="C27" r:id="rId4"/>
-    <hyperlink ref="C34" r:id="rId5"/>
-    <hyperlink ref="C45" r:id="rId6"/>
-    <hyperlink ref="C52" r:id="rId7"/>
-    <hyperlink ref="C59" r:id="rId8"/>
-    <hyperlink ref="C66" r:id="rId9"/>
-    <hyperlink ref="C73" r:id="rId10"/>
-    <hyperlink ref="C80" r:id="rId11"/>
-    <hyperlink ref="C87:C88" r:id="rId12" display="X"/>
-    <hyperlink ref="C21" r:id="rId13"/>
+    <hyperlink ref="C12" r:id="rId2"/>
+    <hyperlink ref="C19" r:id="rId3"/>
+    <hyperlink ref="C26" r:id="rId4"/>
+    <hyperlink ref="C33" r:id="rId5"/>
+    <hyperlink ref="C44" r:id="rId6"/>
+    <hyperlink ref="C51" r:id="rId7"/>
+    <hyperlink ref="C58" r:id="rId8"/>
+    <hyperlink ref="C65" r:id="rId9"/>
+    <hyperlink ref="C72" r:id="rId10"/>
+    <hyperlink ref="C79" r:id="rId11"/>
+    <hyperlink ref="C86:C87" r:id="rId12" display="X"/>
+    <hyperlink ref="C20" r:id="rId13"/>
     <hyperlink ref="C7" r:id="rId14"/>
-    <hyperlink ref="C14" r:id="rId15"/>
-    <hyperlink ref="C35" r:id="rId16"/>
-    <hyperlink ref="D52" r:id="rId17"/>
-    <hyperlink ref="D73" r:id="rId18"/>
-    <hyperlink ref="D88" r:id="rId19"/>
+    <hyperlink ref="C13" r:id="rId15"/>
+    <hyperlink ref="C34" r:id="rId16"/>
+    <hyperlink ref="D72" r:id="rId17"/>
+    <hyperlink ref="D87" r:id="rId18"/>
+    <hyperlink ref="D21" r:id="rId19"/>
+    <hyperlink ref="D14" r:id="rId20"/>
+    <hyperlink ref="D9" r:id="rId21"/>
+    <hyperlink ref="D8" r:id="rId22"/>
+    <hyperlink ref="D45" r:id="rId23"/>
+    <hyperlink ref="D52:D54" r:id="rId24" display="X"/>
+    <hyperlink ref="D59:D60" r:id="rId25" display="X"/>
+    <hyperlink ref="D66" r:id="rId26"/>
+    <hyperlink ref="D73" r:id="rId27"/>
+    <hyperlink ref="D80" r:id="rId28"/>
+    <hyperlink ref="D88" r:id="rId29"/>
+    <hyperlink ref="D27" r:id="rId30"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.49212598499999999" footer="0.49212598499999999"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId20"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId31"/>
   <headerFooter alignWithMargins="0"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
#02 - Avaliação do Projeto
</commit_message>
<xml_diff>
--- a/Processo/Avaliação/GRE-Avaliacao-Projeto.xlsx
+++ b/Processo/Avaliação/GRE-Avaliacao-Projeto.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="55">
   <si>
     <t>INSTRUÇÕES</t>
   </si>
@@ -186,20 +186,6 @@
         <family val="2"/>
       </rPr>
       <t xml:space="preserve">                                                </t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">RAP 5. As informações e os recursos necessários para a execução do processo são identificados e disponibilizados.
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>As evidências apresentadas para este resultado permitem assegurar que foram identificados e disponibilizados os recursos necessários (ex: pessoal, financeiros,hardware/infra-estrutura, software/ferramentas) e as informações necessárias (ex: processos, padrões, modelos, guias) para executar o processo?</t>
     </r>
   </si>
   <si>
@@ -1418,8 +1404,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F126"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G32" sqref="G32"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A28" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1479,7 +1465,7 @@
     </row>
     <row r="6" spans="1:4" ht="12.75">
       <c r="A6" s="48" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B6" s="14"/>
       <c r="C6" s="49" t="s">
@@ -1499,7 +1485,7 @@
     </row>
     <row r="8" spans="1:4" ht="12.75">
       <c r="A8" s="15" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B8" s="14"/>
       <c r="C8" s="14"/>
@@ -1509,13 +1495,11 @@
     </row>
     <row r="9" spans="1:4" ht="12.75">
       <c r="A9" s="15" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B9" s="14"/>
       <c r="C9" s="14"/>
-      <c r="D9" s="49" t="s">
-        <v>19</v>
-      </c>
+      <c r="D9" s="49"/>
     </row>
     <row r="10" spans="1:4" ht="12.75">
       <c r="A10" s="16"/>
@@ -1535,7 +1519,7 @@
     </row>
     <row r="12" spans="1:4" ht="12.75">
       <c r="A12" s="48" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B12" s="47"/>
       <c r="C12" s="49" t="s">
@@ -1545,7 +1529,7 @@
     </row>
     <row r="13" spans="1:4" ht="12.75">
       <c r="A13" s="48" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B13" s="14"/>
       <c r="C13" s="49" t="s">
@@ -1555,13 +1539,11 @@
     </row>
     <row r="14" spans="1:4" ht="12.75">
       <c r="A14" s="15" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B14" s="14"/>
       <c r="C14" s="14"/>
-      <c r="D14" s="49" t="s">
-        <v>19</v>
-      </c>
+      <c r="D14" s="49"/>
     </row>
     <row r="15" spans="1:4" ht="12.75">
       <c r="A15" s="15"/>
@@ -1593,7 +1575,7 @@
     </row>
     <row r="19" spans="1:6" ht="12.75">
       <c r="A19" s="48" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B19" s="14"/>
       <c r="C19" s="49" t="s">
@@ -1614,13 +1596,11 @@
     </row>
     <row r="21" spans="1:6" ht="12.75">
       <c r="A21" s="15" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B21" s="14"/>
       <c r="C21" s="14"/>
-      <c r="D21" s="49" t="s">
-        <v>19</v>
-      </c>
+      <c r="D21" s="49"/>
     </row>
     <row r="22" spans="1:6" ht="12.75">
       <c r="A22" s="15"/>
@@ -1652,7 +1632,7 @@
     </row>
     <row r="26" spans="1:6" ht="12.75">
       <c r="A26" s="48" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B26" s="14"/>
       <c r="C26" s="49" t="s">
@@ -1662,7 +1642,7 @@
     </row>
     <row r="27" spans="1:6" ht="12.75">
       <c r="A27" s="15" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B27" s="14"/>
       <c r="C27" s="14"/>
@@ -1706,7 +1686,7 @@
     </row>
     <row r="33" spans="1:4" ht="12.75">
       <c r="A33" s="48" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B33" s="14"/>
       <c r="C33" s="49" t="s">
@@ -1726,19 +1706,19 @@
     </row>
     <row r="35" spans="1:4" ht="12.75">
       <c r="A35" s="15" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B35" s="14"/>
       <c r="C35" s="14" t="s">
-        <v>43</v>
-      </c>
-      <c r="D35" s="14"/>
+        <v>42</v>
+      </c>
+      <c r="D35" s="49"/>
     </row>
     <row r="36" spans="1:4" ht="12.75">
       <c r="A36" s="15"/>
       <c r="B36" s="14"/>
       <c r="C36" s="14" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D36" s="14"/>
     </row>
@@ -1796,7 +1776,7 @@
     </row>
     <row r="44" spans="1:4" ht="12.75">
       <c r="A44" s="48" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B44" s="14"/>
       <c r="C44" s="49" t="s">
@@ -1806,7 +1786,7 @@
     </row>
     <row r="45" spans="1:4" ht="12.75">
       <c r="A45" s="15" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B45" s="14"/>
       <c r="C45" s="14"/>
@@ -1850,7 +1830,7 @@
     </row>
     <row r="51" spans="1:4" ht="12.75">
       <c r="A51" s="48" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B51" s="14"/>
       <c r="C51" s="50" t="s">
@@ -1860,7 +1840,7 @@
     </row>
     <row r="52" spans="1:4" ht="12.75">
       <c r="A52" s="15" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B52" s="14"/>
       <c r="C52" s="14"/>
@@ -1870,7 +1850,7 @@
     </row>
     <row r="53" spans="1:4" ht="12.75">
       <c r="A53" s="15" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B53" s="14"/>
       <c r="C53" s="14"/>
@@ -1880,7 +1860,7 @@
     </row>
     <row r="54" spans="1:4" ht="12.75">
       <c r="A54" s="15" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B54" s="14"/>
       <c r="C54" s="14"/>
@@ -1902,17 +1882,15 @@
       <c r="C56" s="18"/>
       <c r="D56" s="18"/>
     </row>
-    <row r="57" spans="1:4" ht="64.5">
-      <c r="A57" s="28" t="s">
-        <v>32</v>
-      </c>
+    <row r="57" spans="1:4" ht="15.75">
+      <c r="A57" s="28"/>
       <c r="B57" s="32"/>
       <c r="C57" s="32"/>
       <c r="D57" s="32"/>
     </row>
     <row r="58" spans="1:4" ht="12.75">
       <c r="A58" s="48" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B58" s="14"/>
       <c r="C58" s="49" t="s">
@@ -1922,7 +1900,7 @@
     </row>
     <row r="59" spans="1:4" ht="12.75">
       <c r="A59" s="15" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B59" s="14"/>
       <c r="C59" s="14"/>
@@ -1932,7 +1910,7 @@
     </row>
     <row r="60" spans="1:4" ht="12.75">
       <c r="A60" s="15" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B60" s="14"/>
       <c r="C60" s="14"/>
@@ -1962,7 +1940,7 @@
     </row>
     <row r="64" spans="1:4" ht="51.75">
       <c r="A64" s="28" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B64" s="32"/>
       <c r="C64" s="32"/>
@@ -1970,7 +1948,7 @@
     </row>
     <row r="65" spans="1:4" ht="12.75">
       <c r="A65" s="48" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B65" s="14"/>
       <c r="C65" s="49" t="s">
@@ -1980,7 +1958,7 @@
     </row>
     <row r="66" spans="1:4" ht="12.75">
       <c r="A66" s="15" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B66" s="14"/>
       <c r="C66" s="14"/>
@@ -2016,7 +1994,7 @@
     </row>
     <row r="71" spans="1:4" ht="64.5">
       <c r="A71" s="28" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B71" s="32"/>
       <c r="C71" s="32"/>
@@ -2024,7 +2002,7 @@
     </row>
     <row r="72" spans="1:4" ht="12.75">
       <c r="A72" s="48" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B72" s="14"/>
       <c r="C72" s="49" t="s">
@@ -2036,7 +2014,7 @@
     </row>
     <row r="73" spans="1:4" ht="12.75">
       <c r="A73" s="15" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B73" s="14"/>
       <c r="C73" s="14"/>
@@ -2072,7 +2050,7 @@
     </row>
     <row r="78" spans="1:4" ht="64.5">
       <c r="A78" s="28" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B78" s="32"/>
       <c r="C78" s="32"/>
@@ -2080,7 +2058,7 @@
     </row>
     <row r="79" spans="1:4" ht="12.75">
       <c r="A79" s="48" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B79" s="14"/>
       <c r="C79" s="49" t="s">
@@ -2090,7 +2068,7 @@
     </row>
     <row r="80" spans="1:4" ht="12.75">
       <c r="A80" s="15" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B80" s="14"/>
       <c r="C80" s="14"/>
@@ -2126,7 +2104,7 @@
     </row>
     <row r="85" spans="1:4" ht="51.75">
       <c r="A85" s="28" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B85" s="32"/>
       <c r="C85" s="32"/>
@@ -2134,7 +2112,7 @@
     </row>
     <row r="86" spans="1:4" ht="12.75">
       <c r="A86" s="48" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B86" s="14"/>
       <c r="C86" s="49" t="s">
@@ -2144,7 +2122,7 @@
     </row>
     <row r="87" spans="1:4" ht="12.75">
       <c r="A87" s="48" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B87" s="14"/>
       <c r="C87" s="49" t="s">
@@ -2156,7 +2134,7 @@
     </row>
     <row r="88" spans="1:4" ht="12.75">
       <c r="A88" s="15" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B88" s="14"/>
       <c r="C88" s="14"/>
@@ -2415,21 +2393,18 @@
     <hyperlink ref="C34" r:id="rId16"/>
     <hyperlink ref="D72" r:id="rId17"/>
     <hyperlink ref="D87" r:id="rId18"/>
-    <hyperlink ref="D21" r:id="rId19"/>
-    <hyperlink ref="D14" r:id="rId20"/>
-    <hyperlink ref="D9" r:id="rId21"/>
-    <hyperlink ref="D8" r:id="rId22"/>
-    <hyperlink ref="D45" r:id="rId23"/>
-    <hyperlink ref="D52:D54" r:id="rId24" display="X"/>
-    <hyperlink ref="D59:D60" r:id="rId25" display="X"/>
-    <hyperlink ref="D66" r:id="rId26"/>
-    <hyperlink ref="D73" r:id="rId27"/>
-    <hyperlink ref="D80" r:id="rId28"/>
-    <hyperlink ref="D88" r:id="rId29"/>
-    <hyperlink ref="D27" r:id="rId30"/>
+    <hyperlink ref="D45" r:id="rId19"/>
+    <hyperlink ref="D52:D54" r:id="rId20" display="X"/>
+    <hyperlink ref="D59:D60" r:id="rId21" display="X"/>
+    <hyperlink ref="D66" r:id="rId22"/>
+    <hyperlink ref="D73" r:id="rId23"/>
+    <hyperlink ref="D80" r:id="rId24"/>
+    <hyperlink ref="D88" r:id="rId25"/>
+    <hyperlink ref="D27" r:id="rId26"/>
+    <hyperlink ref="D8" r:id="rId27"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.49212598499999999" footer="0.49212598499999999"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId31"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId28"/>
   <headerFooter alignWithMargins="0"/>
 </worksheet>
 </file>
</xml_diff>